<commit_message>
Arreglé las columnas que quedaban como triángulos
</commit_message>
<xml_diff>
--- a/datasets/rm_22_23.xlsx
+++ b/datasets/rm_22_23.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fryep\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\franciscayepsen\s2_25\mineria_datos\proyecto-mineria-de-datos\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9690" windowHeight="6795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8235"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="244">
   <si>
-    <t>▲</t>
-  </si>
-  <si>
     <t>Nation</t>
   </si>
   <si>
@@ -756,6 +753,9 @@
   </si>
   <si>
     <t>1.65</t>
+  </si>
+  <si>
+    <t>Player</t>
   </si>
 </sst>
 </file>
@@ -1391,9 +1391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G1:G1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1402,117 +1400,117 @@
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
-        <v>0</v>
+        <v>243</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="P1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="W1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="X1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z1" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AC1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AF1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AG1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="10" t="s">
+      <c r="AH1" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH1" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="2">
         <v>30</v>
@@ -1527,7 +1525,7 @@
         <v>1838</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I2" s="3">
         <v>1</v>
@@ -1554,16 +1552,16 @@
         <v>0</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="U2" s="3">
         <v>16</v>
@@ -1575,48 +1573,48 @@
         <v>60</v>
       </c>
       <c r="X2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AG2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AD2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="AH2" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D3" s="2">
         <v>20</v>
@@ -1631,43 +1629,43 @@
         <v>19</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="4">
-        <v>0</v>
-      </c>
-      <c r="K3" s="4">
-        <v>0</v>
-      </c>
-      <c r="L3" s="4">
-        <v>0</v>
-      </c>
-      <c r="M3" s="4">
-        <v>0</v>
-      </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
-        <v>0</v>
-      </c>
-      <c r="P3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S3" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="T3" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U3" s="3">
         <v>0</v>
@@ -1679,48 +1677,48 @@
         <v>0</v>
       </c>
       <c r="X3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="AD3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Z3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AE3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG3" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="AH3" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D4" s="2">
         <v>26</v>
@@ -1735,7 +1733,7 @@
         <v>1442</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I4" s="3">
         <v>9</v>
@@ -1762,16 +1760,16 @@
         <v>0</v>
       </c>
       <c r="Q4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="S4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="T4" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="U4" s="3">
         <v>56</v>
@@ -1783,48 +1781,48 @@
         <v>108</v>
       </c>
       <c r="X4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y4" s="4" t="s">
+      <c r="Z4" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="Z4" s="4" t="s">
+      <c r="AA4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AA4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC4" s="3" t="s">
+      <c r="AD4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AD4" s="4" t="s">
+      <c r="AE4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AE4" s="4" t="s">
+      <c r="AF4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AF4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AG4" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="AH4" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="D5" s="2">
         <v>34</v>
@@ -1839,7 +1837,7 @@
         <v>2038</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5" s="3">
         <v>19</v>
@@ -1866,16 +1864,16 @@
         <v>0</v>
       </c>
       <c r="Q5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="R5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="T5" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="T5" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="U5" s="3">
         <v>72</v>
@@ -1887,48 +1885,48 @@
         <v>157</v>
       </c>
       <c r="X5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AD5" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AG5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="AF5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>78</v>
-      </c>
       <c r="AH5" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D6" s="2">
         <v>19</v>
@@ -1943,7 +1941,7 @@
         <v>201</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="3">
         <v>0</v>
@@ -1970,16 +1968,16 @@
         <v>0</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S6" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="T6" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="U6" s="3">
         <v>69</v>
@@ -1991,48 +1989,48 @@
         <v>99</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AD6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE6" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AE6" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="AF6" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AG6" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH6" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D7" s="2">
         <v>20</v>
@@ -2071,18 +2069,18 @@
       <c r="AF7" s="4"/>
       <c r="AG7" s="4"/>
       <c r="AH7" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2">
         <v>30</v>
@@ -2097,7 +2095,7 @@
         <v>1784</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I8" s="3">
         <v>0</v>
@@ -2124,16 +2122,16 @@
         <v>1</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="T8" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="U8" s="3">
         <v>22</v>
@@ -2145,48 +2143,48 @@
         <v>147</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AC8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AD8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AF8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AG8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AH8" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="D9" s="2">
         <v>30</v>
@@ -2201,7 +2199,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I9" s="3">
         <v>0</v>
@@ -2228,16 +2226,16 @@
         <v>0</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U9" s="3">
         <v>0</v>
@@ -2249,48 +2247,48 @@
         <v>0</v>
       </c>
       <c r="X9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AD9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AF9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH9" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="2">
         <v>25</v>
@@ -2305,7 +2303,7 @@
         <v>1564</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I10" s="3">
         <v>0</v>
@@ -2332,16 +2330,16 @@
         <v>0</v>
       </c>
       <c r="Q10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="S10" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="R10" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="S10" s="4" t="s">
+      <c r="T10" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="U10" s="3">
         <v>60</v>
@@ -2353,48 +2351,48 @@
         <v>60</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="Z10" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB10" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD10" s="4" t="s">
+      <c r="AE10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AE10" s="4" t="s">
-        <v>103</v>
-      </c>
       <c r="AF10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH10" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="2">
         <v>30</v>
@@ -2409,96 +2407,96 @@
         <v>279</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S11" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="3">
-        <v>0</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0</v>
-      </c>
-      <c r="P11" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="S11" s="4" t="s">
+      <c r="T11" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0</v>
+      </c>
+      <c r="V11" s="4">
+        <v>0</v>
+      </c>
+      <c r="W11" s="4">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="T11" s="4" t="s">
+      <c r="AE11" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="U11" s="3">
-        <v>0</v>
-      </c>
-      <c r="V11" s="4">
-        <v>0</v>
-      </c>
-      <c r="W11" s="4">
-        <v>0</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AD11" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE11" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="AF11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG11" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AH11" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="2">
         <v>21</v>
@@ -2537,18 +2535,18 @@
       <c r="AF12" s="4"/>
       <c r="AG12" s="4"/>
       <c r="AH12" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2">
         <v>23</v>
@@ -2587,18 +2585,18 @@
       <c r="AF13" s="4"/>
       <c r="AG13" s="4"/>
       <c r="AH13" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2">
         <v>31</v>
@@ -2613,7 +2611,7 @@
         <v>196</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="3">
         <v>0</v>
@@ -2640,16 +2638,16 @@
         <v>0</v>
       </c>
       <c r="Q14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="S14" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="S14" s="4" t="s">
+      <c r="T14" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="T14" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="U14" s="3">
         <v>6</v>
@@ -2661,48 +2659,48 @@
         <v>25</v>
       </c>
       <c r="X14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC14" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="Z14" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB14" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC14" s="3" t="s">
+      <c r="AD14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE14" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="AD14" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE14" s="4" t="s">
+      <c r="AF14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="AF14" s="4" t="s">
+      <c r="AG14" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="AG14" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="AH14" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="2">
         <v>22</v>
@@ -2717,7 +2715,7 @@
         <v>2823</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I15" s="3">
         <v>10</v>
@@ -2744,16 +2742,16 @@
         <v>1</v>
       </c>
       <c r="Q15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="S15" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="R15" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="S15" s="4" t="s">
+      <c r="T15" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>125</v>
       </c>
       <c r="U15" s="3">
         <v>221</v>
@@ -2765,48 +2763,48 @@
         <v>495</v>
       </c>
       <c r="X15" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y15" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Y15" s="4" t="s">
+      <c r="Z15" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Z15" s="4" t="s">
+      <c r="AA15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC15" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="AA15" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AB15" s="4" t="s">
+      <c r="AD15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AF15" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AC15" s="3" t="s">
+      <c r="AG15" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="AD15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG15" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="AH15" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D16" s="2">
         <v>32</v>
@@ -2821,7 +2819,7 @@
         <v>2155</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I16" s="3">
         <v>2</v>
@@ -2848,16 +2846,16 @@
         <v>1</v>
       </c>
       <c r="Q16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="S16" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="R16" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="S16" s="4" t="s">
+      <c r="T16" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="T16" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="U16" s="3">
         <v>51</v>
@@ -2869,48 +2867,48 @@
         <v>38</v>
       </c>
       <c r="X16" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y16" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Z16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB16" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC16" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="AA16" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AB16" s="4" t="s">
+      <c r="AD16" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF16" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="AC16" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD16" s="4" t="s">
+      <c r="AG16" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="AE16" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="AG16" s="4" t="s">
-        <v>140</v>
-      </c>
       <c r="AH16" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="2">
         <v>21</v>
@@ -2949,18 +2947,18 @@
       <c r="AF17" s="4"/>
       <c r="AG17" s="4"/>
       <c r="AH17" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="2">
         <v>20</v>
@@ -2999,18 +2997,18 @@
       <c r="AF18" s="4"/>
       <c r="AG18" s="4"/>
       <c r="AH18" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="2">
         <v>23</v>
@@ -3025,7 +3023,7 @@
         <v>630</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I19" s="3">
         <v>0</v>
@@ -3052,16 +3050,16 @@
         <v>0</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U19" s="3">
         <v>0</v>
@@ -3073,48 +3071,48 @@
         <v>0</v>
       </c>
       <c r="X19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AD19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AF19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AG19" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AH19" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="2">
         <v>28</v>
@@ -3129,7 +3127,7 @@
         <v>157</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I20" s="3">
         <v>0</v>
@@ -3156,16 +3154,16 @@
         <v>0</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U20" s="3">
         <v>3</v>
@@ -3177,48 +3175,48 @@
         <v>12</v>
       </c>
       <c r="X20" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB20" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC20" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AD20" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AE20" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AF20" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AG20" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="AH20" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="2">
         <v>18</v>
@@ -3257,18 +3255,18 @@
       <c r="AF21" s="4"/>
       <c r="AG21" s="4"/>
       <c r="AH21" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2">
         <v>27</v>
@@ -3283,7 +3281,7 @@
         <v>1351</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I22" s="3">
         <v>0</v>
@@ -3310,16 +3308,16 @@
         <v>0</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="U22" s="3">
         <v>23</v>
@@ -3331,48 +3329,48 @@
         <v>73</v>
       </c>
       <c r="X22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Z22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB22" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AC22" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AD22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AE22" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AF22" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AG22" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="AH22" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2">
         <v>24</v>
@@ -3387,7 +3385,7 @@
         <v>2703</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I23" s="3">
         <v>5</v>
@@ -3414,16 +3412,16 @@
         <v>0</v>
       </c>
       <c r="Q23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="S23" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="T23" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="R23" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="T23" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="U23" s="3">
         <v>28</v>
@@ -3435,48 +3433,48 @@
         <v>16</v>
       </c>
       <c r="X23" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z23" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA23" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AB23" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AC23" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD23" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AE23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AF23" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AG23" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AH23" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="2">
         <v>36</v>
@@ -3491,7 +3489,7 @@
         <v>1744</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I24" s="3">
         <v>4</v>
@@ -3518,16 +3516,16 @@
         <v>0</v>
       </c>
       <c r="Q24" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="R24" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="R24" s="4" t="s">
+      <c r="S24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="S24" s="4" t="s">
+      <c r="T24" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>166</v>
       </c>
       <c r="U24" s="3">
         <v>50</v>
@@ -3539,48 +3537,48 @@
         <v>87</v>
       </c>
       <c r="X24" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z24" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="Y24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z24" s="4" t="s">
+      <c r="AA24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB24" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC24" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="AA24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB24" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC24" s="3" t="s">
+      <c r="AD24" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AF24" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="AD24" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE24" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF24" s="4" t="s">
+      <c r="AG24" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="AG24" s="4" t="s">
-        <v>171</v>
-      </c>
       <c r="AH24" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2">
         <v>32</v>
@@ -3595,7 +3593,7 @@
         <v>1637</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I25" s="3">
         <v>1</v>
@@ -3622,16 +3620,16 @@
         <v>0</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="U25" s="3">
         <v>18</v>
@@ -3643,48 +3641,48 @@
         <v>34</v>
       </c>
       <c r="X25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AA25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB25" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AC25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AD25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE25" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="AF25" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AG25" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="AH25" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2">
         <v>26</v>
@@ -3699,7 +3697,7 @@
         <v>39</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
@@ -3726,16 +3724,16 @@
         <v>0</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U26" s="3">
         <v>4</v>
@@ -3747,48 +3745,48 @@
         <v>5</v>
       </c>
       <c r="X26" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB26" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC26" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AD26" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AE26" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AF26" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AG26" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AH26" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="C27" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D27" s="2">
         <v>17</v>
@@ -3827,18 +3825,18 @@
       <c r="AF27" s="4"/>
       <c r="AG27" s="4"/>
       <c r="AH27" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="2">
         <v>18</v>
@@ -3877,18 +3875,18 @@
       <c r="AF28" s="4"/>
       <c r="AG28" s="4"/>
       <c r="AH28" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>181</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="2">
         <v>18</v>
@@ -3903,7 +3901,7 @@
         <v>79</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I29" s="3">
         <v>1</v>
@@ -3930,16 +3928,16 @@
         <v>0</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U29" s="3">
         <v>0</v>
@@ -3951,48 +3949,48 @@
         <v>3</v>
       </c>
       <c r="X29" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y29" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Z29" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="Y29" s="4" t="s">
+      <c r="AA29" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB29" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="Z29" s="4" t="s">
+      <c r="AC29" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="AA29" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AB29" s="4" t="s">
+      <c r="AD29" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE29" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF29" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="AC29" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="AD29" s="4" t="s">
+      <c r="AG29" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="AE29" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="AF29" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="AG29" s="4" t="s">
-        <v>186</v>
-      </c>
       <c r="AH29" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="2">
         <v>21</v>
@@ -4007,7 +4005,7 @@
         <v>2379</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I30" s="3">
         <v>9</v>
@@ -4034,16 +4032,16 @@
         <v>0</v>
       </c>
       <c r="Q30" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="R30" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="R30" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="S30" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T30" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="U30" s="3">
         <v>146</v>
@@ -4055,48 +4053,48 @@
         <v>268</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z30" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AA30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB30" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC30" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AA30" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AB30" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC30" s="3" t="s">
+      <c r="AD30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE30" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AD30" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE30" s="4" t="s">
+      <c r="AF30" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="AF30" s="4" t="s">
+      <c r="AG30" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AG30" s="4" t="s">
-        <v>195</v>
-      </c>
       <c r="AH30" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2">
         <v>29</v>
@@ -4111,7 +4109,7 @@
         <v>2415</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I31" s="3">
         <v>1</v>
@@ -4138,16 +4136,16 @@
         <v>0</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="U31" s="3">
         <v>21</v>
@@ -4159,48 +4157,48 @@
         <v>10</v>
       </c>
       <c r="X31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AB31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AC31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AD31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AF31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AG31" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AH31" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D32" s="2">
         <v>22</v>
@@ -4215,7 +4213,7 @@
         <v>2119</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I32" s="3">
         <v>0</v>
@@ -4242,16 +4240,16 @@
         <v>0</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S32" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T32" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U32" s="3">
         <v>41</v>
@@ -4263,48 +4261,48 @@
         <v>23</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Z32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA32" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AC32" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AD32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AE32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AF32" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AG32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH32" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="2">
         <v>25</v>
@@ -4319,43 +4317,43 @@
         <v>22</v>
       </c>
       <c r="H33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="4">
+        <v>0</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4">
+        <v>0</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <v>0</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0</v>
+      </c>
+      <c r="P33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="S33" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="I33" s="3">
-        <v>0</v>
-      </c>
-      <c r="J33" s="4">
-        <v>0</v>
-      </c>
-      <c r="K33" s="4">
-        <v>0</v>
-      </c>
-      <c r="L33" s="4">
-        <v>0</v>
-      </c>
-      <c r="M33" s="4">
-        <v>0</v>
-      </c>
-      <c r="N33" s="4">
-        <v>0</v>
-      </c>
-      <c r="O33" s="4">
-        <v>0</v>
-      </c>
-      <c r="P33" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q33" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="S33" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="T33" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U33" s="3">
         <v>0</v>
@@ -4367,48 +4365,48 @@
         <v>0</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Y33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Z33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AA33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AB33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC33" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AD33" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AE33" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AF33" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AG33" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="AH33" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2">
         <v>24</v>
@@ -4423,7 +4421,7 @@
         <v>2502</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I34" s="3">
         <v>7</v>
@@ -4450,16 +4448,16 @@
         <v>0</v>
       </c>
       <c r="Q34" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="T34" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="S34" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="T34" s="4" t="s">
-        <v>207</v>
       </c>
       <c r="U34" s="3">
         <v>70</v>
@@ -4471,48 +4469,48 @@
         <v>135</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Y34" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Z34" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA34" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB34" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AC34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE34" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="AA34" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="AB34" s="4" t="s">
+      <c r="AF34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG34" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="AC34" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD34" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE34" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="AF34" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG34" s="4" t="s">
-        <v>209</v>
-      </c>
       <c r="AH34" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="2">
         <v>31</v>
@@ -4527,7 +4525,7 @@
         <v>1144</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I35" s="3">
         <v>4</v>
@@ -4554,16 +4552,16 @@
         <v>0</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S35" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="T35" s="4" t="s">
         <v>212</v>
-      </c>
-      <c r="T35" s="4" t="s">
-        <v>213</v>
       </c>
       <c r="U35" s="3">
         <v>31</v>
@@ -4575,47 +4573,47 @@
         <v>145</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y35" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z35" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA35" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="Z35" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA35" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="AB35" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC35" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AE35" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF35" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG35" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AH35" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B36" s="5"/>
       <c r="C36" s="6"/>
       <c r="D36" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E36" s="7">
         <v>38</v>
@@ -4627,7 +4625,7 @@
         <v>342</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I36" s="7">
         <v>73</v>
@@ -4654,16 +4652,16 @@
         <v>3</v>
       </c>
       <c r="Q36" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="R36" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="R36" s="8" t="s">
+      <c r="S36" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="S36" s="8" t="s">
+      <c r="T36" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="T36" s="8" t="s">
-        <v>220</v>
       </c>
       <c r="U36" s="7">
         <v>1008</v>
@@ -4675,45 +4673,45 @@
         <v>2000</v>
       </c>
       <c r="X36" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y36" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="Y36" s="8" t="s">
+      <c r="Z36" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="Z36" s="8" t="s">
+      <c r="AA36" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="AA36" s="8" t="s">
+      <c r="AB36" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="AB36" s="8" t="s">
+      <c r="AC36" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="AC36" s="7" t="s">
+      <c r="AD36" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="AD36" s="8" t="s">
+      <c r="AE36" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AE36" s="8" t="s">
+      <c r="AF36" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="AF36" s="8" t="s">
+      <c r="AG36" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="AG36" s="8" t="s">
-        <v>230</v>
       </c>
       <c r="AH36" s="17"/>
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
       <c r="D37" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E37" s="21">
         <v>38</v>
@@ -4725,7 +4723,7 @@
         <v>342</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I37" s="21">
         <v>35</v>
@@ -4752,16 +4750,16 @@
         <v>7</v>
       </c>
       <c r="Q37" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="R37" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="R37" s="22" t="s">
+      <c r="S37" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="T37" s="22" t="s">
         <v>234</v>
-      </c>
-      <c r="S37" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="T37" s="22" t="s">
-        <v>235</v>
       </c>
       <c r="U37" s="21">
         <v>631</v>
@@ -4773,34 +4771,34 @@
         <v>1178</v>
       </c>
       <c r="X37" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y37" s="22" t="s">
         <v>236</v>
       </c>
-      <c r="Y37" s="22" t="s">
+      <c r="Z37" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA37" s="22" t="s">
         <v>237</v>
       </c>
-      <c r="Z37" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="AA37" s="22" t="s">
+      <c r="AB37" s="22" t="s">
         <v>238</v>
       </c>
-      <c r="AB37" s="22" t="s">
+      <c r="AC37" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="AC37" s="21" t="s">
+      <c r="AD37" s="22" t="s">
         <v>240</v>
       </c>
-      <c r="AD37" s="22" t="s">
+      <c r="AE37" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="AE37" s="22" t="s">
+      <c r="AF37" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG37" s="22" t="s">
         <v>242</v>
-      </c>
-      <c r="AF37" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="AG37" s="22" t="s">
-        <v>243</v>
       </c>
       <c r="AH37" s="23"/>
     </row>
@@ -4902,5 +4900,6 @@
     <hyperlink ref="AH35" r:id="rId94" display="https://fbref.com/en/players/fd51b456/matchlogs/2022-2023/summary/Lucas-Vazquez-Match-Logs"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId95"/>
 </worksheet>
 </file>
</xml_diff>